<commit_message>
Changed poop and lerned pewp
</commit_message>
<xml_diff>
--- a/Star Data.xlsx
+++ b/Star Data.xlsx
@@ -77,9 +77,6 @@
     <t>Luminosity(Lsun)(Log10)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Log10R Radius (RSun)(Log10)</t>
-  </si>
-  <si>
     <t>Touter (Log10)</t>
   </si>
   <si>
@@ -148,12 +145,15 @@
   <si>
     <t>Radius of oxygen core (R☉)</t>
   </si>
+  <si>
+    <t>Radius (RSun)(Log10)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +293,13 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -664,8 +671,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -997,25 +1004,41 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="5" width="9" customWidth="1"/>
-    <col min="6" max="9" width="8.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" customWidth="1"/>
-    <col min="12" max="15" width="8.28515625" customWidth="1"/>
-    <col min="16" max="21" width="8.5703125" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" customWidth="1"/>
-    <col min="23" max="23" width="8.5703125" customWidth="1"/>
-    <col min="24" max="29" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="27.5703125" customWidth="1"/>
+    <col min="18" max="18" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1029,79 +1052,79 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>